<commit_message>
Fix some bug in FitnessFunc & set Debug mode in OSS2Params
</commit_message>
<xml_diff>
--- a/jaea/kkydata/KKY-bounds.xlsx
+++ b/jaea/kkydata/KKY-bounds.xlsx
@@ -428,7 +428,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:S27"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -445,7 +445,7 @@
         <v>19</v>
       </c>
       <c r="G1">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -460,20 +460,20 @@
       </c>
       <c r="F2">
         <f>$A2-$G$1*ABS($A2)</f>
-        <v>-1.6560000000000001</v>
+        <v>-1.1040000000000001</v>
       </c>
       <c r="G2">
         <f>$A2+$G$1*ABS($A2)</f>
-        <v>-0.18399999999999994</v>
+        <v>-0.73599999999999999</v>
       </c>
       <c r="L2">
         <v>0.5</v>
       </c>
       <c r="N2">
-        <v>-1.6560000000000001</v>
+        <v>-1.1040000000000001</v>
       </c>
       <c r="O2">
-        <v>-0.18399999999999994</v>
+        <v>-0.73599999999999999</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -494,20 +494,20 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F20" si="0">$A3-$G$1*ABS($A3)</f>
-        <v>0.34559999999999991</v>
+        <v>1.3824000000000001</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G20" si="1">$A3+$G$1*ABS($A3)</f>
-        <v>3.1104000000000003</v>
+        <v>2.0735999999999999</v>
       </c>
       <c r="L3">
         <v>0.5</v>
       </c>
       <c r="N3">
-        <v>0.34559999999999991</v>
+        <v>1.3824000000000001</v>
       </c>
       <c r="O3">
-        <v>3.1104000000000003</v>
+        <v>2.0735999999999999</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -528,20 +528,20 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>2.5499999999999995E-2</v>
+        <v>0.10200000000000001</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>0.22950000000000001</v>
+        <v>0.153</v>
       </c>
       <c r="L4">
         <v>0.5</v>
       </c>
       <c r="N4">
-        <v>2.5499999999999995E-2</v>
+        <v>0.10200000000000001</v>
       </c>
       <c r="O4">
-        <v>0.22950000000000001</v>
+        <v>0.153</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -562,20 +562,20 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>11.211999999999996</v>
+        <v>44.847999999999999</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>100.90800000000002</v>
+        <v>67.272000000000006</v>
       </c>
       <c r="L5">
         <v>0.5</v>
       </c>
       <c r="N5">
-        <v>11.211999999999996</v>
+        <v>44.847999999999999</v>
       </c>
       <c r="O5">
-        <v>100.90800000000002</v>
+        <v>67.272000000000006</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -596,20 +596,20 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>9.1999999999999971E-2</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>0.82800000000000007</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="L6">
         <v>0.5</v>
       </c>
       <c r="N6">
-        <v>9.1999999999999971E-2</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="O6">
-        <v>0.82800000000000007</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -630,20 +630,20 @@
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>6.9999999999999993E-3</v>
+        <v>2.8000000000000004E-2</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>6.3E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="L7">
         <v>0.5</v>
       </c>
       <c r="N7">
-        <v>6.9999999999999993E-3</v>
+        <v>2.8000000000000004E-2</v>
       </c>
       <c r="O7">
-        <v>6.3E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -664,20 +664,20 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>8.7999999999999953E-3</v>
+        <v>3.5199999999999995E-2</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>7.9199999999999993E-2</v>
+        <v>5.28E-2</v>
       </c>
       <c r="L8">
         <v>0.5</v>
       </c>
       <c r="N8">
-        <v>8.7999999999999953E-3</v>
+        <v>3.5199999999999995E-2</v>
       </c>
       <c r="O8">
-        <v>7.9199999999999993E-2</v>
+        <v>5.28E-2</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -732,20 +732,20 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>11478.985999999997</v>
+        <v>45915.944000000003</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>103310.87400000001</v>
+        <v>68873.915999999997</v>
       </c>
       <c r="L10">
         <v>0.5</v>
       </c>
       <c r="N10">
-        <v>11478.985999999997</v>
+        <v>45915.944000000003</v>
       </c>
       <c r="O10">
-        <v>103310.87400000001</v>
+        <v>68873.915999999997</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -766,20 +766,20 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>1.4799999999999995</v>
+        <v>5.92</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>13.32</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="L11">
         <v>0.5</v>
       </c>
       <c r="N11">
-        <v>1.4799999999999995</v>
+        <v>5.92</v>
       </c>
       <c r="O11">
-        <v>13.32</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -800,20 +800,20 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>-3940.7400000000007</v>
+        <v>-2627.1600000000003</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>-437.8599999999999</v>
+        <v>-1751.44</v>
       </c>
       <c r="L12">
         <v>0.5</v>
       </c>
       <c r="N12">
-        <v>-3940.7400000000007</v>
+        <v>-2627.1600000000003</v>
       </c>
       <c r="O12">
-        <v>-437.8599999999999</v>
+        <v>-1751.44</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -834,20 +834,20 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0.62599999999999989</v>
+        <v>2.504</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>5.6340000000000003</v>
+        <v>3.7559999999999998</v>
       </c>
       <c r="L13">
         <v>0.5</v>
       </c>
       <c r="N13">
-        <v>0.62599999999999989</v>
+        <v>2.504</v>
       </c>
       <c r="O13">
-        <v>5.6340000000000003</v>
+        <v>3.7559999999999998</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -868,20 +868,20 @@
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>6.9480000000000004</v>
+        <v>27.792000000000002</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>62.532000000000004</v>
+        <v>41.688000000000002</v>
       </c>
       <c r="L14">
         <v>0.5</v>
       </c>
       <c r="N14">
-        <v>6.9480000000000004</v>
+        <v>27.792000000000002</v>
       </c>
       <c r="O14">
-        <v>62.532000000000004</v>
+        <v>41.688000000000002</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -902,20 +902,20 @@
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>2.5599999999999987</v>
+        <v>10.24</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>23.040000000000003</v>
+        <v>15.360000000000001</v>
       </c>
       <c r="L15">
         <v>0.5</v>
       </c>
       <c r="N15">
-        <v>2.5599999999999987</v>
+        <v>10.24</v>
       </c>
       <c r="O15">
-        <v>23.040000000000003</v>
+        <v>15.360000000000001</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -936,20 +936,20 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>0.25659999999999994</v>
+        <v>1.0264</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>2.3094000000000001</v>
+        <v>1.5395999999999999</v>
       </c>
       <c r="L16">
         <v>0.5</v>
       </c>
       <c r="N16">
-        <v>0.25659999999999994</v>
+        <v>1.0264</v>
       </c>
       <c r="O16">
-        <v>2.3094000000000001</v>
+        <v>1.5395999999999999</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -970,20 +970,20 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>13.8506</v>
+        <v>55.4024</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>124.6554</v>
+        <v>83.1036</v>
       </c>
       <c r="L17">
         <v>0.5</v>
       </c>
       <c r="N17">
-        <v>13.8506</v>
+        <v>55.4024</v>
       </c>
       <c r="O17">
-        <v>124.6554</v>
+        <v>83.1036</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -1004,20 +1004,20 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>19.899999999999991</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>179.10000000000002</v>
+        <v>119.4</v>
       </c>
       <c r="L18">
         <v>0.5</v>
       </c>
       <c r="N18">
-        <v>19.899999999999991</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="O18">
-        <v>179.10000000000002</v>
+        <v>119.4</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -1038,20 +1038,20 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>0.28600000000000003</v>
+        <v>1.1439999999999999</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>2.5739999999999998</v>
+        <v>1.716</v>
       </c>
       <c r="L19">
         <v>0.5</v>
       </c>
       <c r="N19">
-        <v>0.28600000000000003</v>
+        <v>1.1439999999999999</v>
       </c>
       <c r="O19">
-        <v>2.5739999999999998</v>
+        <v>1.716</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -1072,20 +1072,20 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>1.8399999999999999</v>
+        <v>7.3599999999999994</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>16.559999999999999</v>
+        <v>11.04</v>
       </c>
       <c r="L20">
         <v>0.5</v>
       </c>
       <c r="N20">
-        <v>1.8399999999999999</v>
+        <v>7.3599999999999994</v>
       </c>
       <c r="O20">
-        <v>16.559999999999999</v>
+        <v>11.04</v>
       </c>
       <c r="P20">
         <v>0</v>

</xml_diff>